<commit_message>
Arreglar problema de carga
</commit_message>
<xml_diff>
--- a/backendHappyPockets/src/main/java/com/happyPockets/service/usuarios.xlsx
+++ b/backendHappyPockets/src/main/java/com/happyPockets/service/usuarios.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\proyecto-IS\backendHappyPockets\src\main\java\com\happyPockets\service\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge\Dev-offline\iis\backendHappyPockets\src\main\java\com\happyPockets\service\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E0893B-B690-4B2E-B295-9C1D60D514EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F79B26-FF69-4DAE-9B5F-D08A815F6DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3996" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{A5FDF81B-2D84-445F-8552-85FD48BFE141}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{A5FDF81B-2D84-445F-8552-85FD48BFE141}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t>Username</t>
   </si>
@@ -63,12 +63,19 @@
   </si>
   <si>
     <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>test1234</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -434,61 +441,84 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{840CBCE0-B017-42F4-BF81-0430A436564B}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.1328125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2">
+      <c r="D2" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="G2" s="0">
         <v>651274927</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="G3" t="n" s="0">
+        <v>123456.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>